<commit_message>
functional Matches validation changed
</commit_message>
<xml_diff>
--- a/test/input/CompanyFiscalYearAndOneSheet.xlsx
+++ b/test/input/CompanyFiscalYearAndOneSheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="96">
   <si>
     <t>Input Value</t>
   </si>
@@ -251,15 +251,6 @@
   </si>
   <si>
     <t>ExTi1</t>
-  </si>
-  <si>
-    <t>CAO</t>
-  </si>
-  <si>
-    <t>COO</t>
-  </si>
-  <si>
-    <t>CEO</t>
   </si>
   <si>
     <t>lala</t>
@@ -706,17 +697,17 @@
   </sheetPr>
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="C41" activeCellId="0" pane="topLeft" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4509803921569"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7725490196078"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -994,7 +985,9 @@
       <c r="B26" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="19" t="n">
+        <v>40971</v>
+      </c>
       <c r="D26" s="23"/>
       <c r="E26" s="24"/>
     </row>
@@ -1127,7 +1120,9 @@
       <c r="B41" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="19" t="n">
+        <v>40971</v>
+      </c>
       <c r="D41" s="23"/>
       <c r="E41" s="24"/>
     </row>
@@ -1409,11 +1404,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C41 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.43137254901961"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1433,42 +1428,42 @@
   </sheetPr>
   <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="N1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="T3" activeCellId="0" pane="topLeft" sqref="T3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="F4" activeCellId="1" pane="topLeft" sqref="C41 F4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8705882352941"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.21960784313726"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.84705882352941"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.74901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6509803921569"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.9960784313726"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.08235294117647"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1058823529412"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9686274509804"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4274509803922"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1058823529412"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.7764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.0196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.09803921568627"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1254901960784"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9921568627451"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1254901960784"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.7960784313726"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.74117647058824"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.24705882352941"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="4.69019607843137"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1529411764706"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1764705882353"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.71764705882353"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2705882352941"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2901960784314"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.71764705882353"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.91764705882353"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.7921568627451"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9764705882353"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.4313725490196"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="11.2666666666667"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.0039215686275"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.443137254902"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="11.278431372549"/>
     <col collapsed="false" hidden="false" max="37" min="32" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="28.0901960784314"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="28.1294117647059"/>
     <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
@@ -1666,17 +1661,11 @@
       <c r="D4" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="I4" s="38" t="n">
         <v>1000</v>
@@ -1748,12 +1737,12 @@
         <v>500</v>
       </c>
       <c r="AL4" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="5">
       <c r="A5" s="36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
@@ -1786,12 +1775,12 @@
       <c r="AD5" s="39"/>
       <c r="AE5" s="39"/>
       <c r="AL5" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="6">
       <c r="A6" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="39"/>
@@ -1824,7 +1813,7 @@
       <c r="AD6" s="39"/>
       <c r="AE6" s="39"/>
       <c r="AL6" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="7">
@@ -1862,12 +1851,12 @@
       <c r="AD7" s="39"/>
       <c r="AE7" s="39"/>
       <c r="AL7" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="8">
       <c r="A8" s="36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -1900,7 +1889,7 @@
       <c r="AD8" s="39"/>
       <c r="AE8" s="39"/>
       <c r="AL8" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="9">
@@ -1911,7 +1900,7 @@
       <c r="AD9" s="39"/>
       <c r="AE9" s="39"/>
       <c r="AL9" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="10">
@@ -1919,25 +1908,19 @@
         <v>74</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="I10" s="38" t="n">
         <v>1000</v>
@@ -2009,12 +1992,12 @@
         <v>500</v>
       </c>
       <c r="AL10" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="11">
       <c r="A11" s="36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -2047,12 +2030,12 @@
       <c r="AD11" s="39"/>
       <c r="AE11" s="39"/>
       <c r="AL11" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="12">
       <c r="A12" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -2085,7 +2068,7 @@
       <c r="AD12" s="39"/>
       <c r="AE12" s="39"/>
       <c r="AL12" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="13">
@@ -2123,12 +2106,12 @@
       <c r="AD13" s="39"/>
       <c r="AE13" s="39"/>
       <c r="AL13" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="14">
       <c r="A14" s="36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -2161,7 +2144,7 @@
       <c r="AD14" s="39"/>
       <c r="AE14" s="39"/>
       <c r="AL14" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Query exported to excel
</commit_message>
<xml_diff>
--- a/test/input/CompanyFiscalYearAndOneSheet.xlsx
+++ b/test/input/CompanyFiscalYearAndOneSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="5" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="133" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>Input Value</t>
   </si>
@@ -195,7 +195,7 @@
     <t>BS%</t>
   </si>
   <si>
-    <t>Time-Vest RS Value</t>
+    <t>TimeVestRsValue</t>
   </si>
   <si>
     <t>Shares</t>
@@ -528,19 +528,19 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.478431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -552,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2" s="2">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2" s="2">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,7 +564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -579,7 +579,7 @@
       </c>
       <c r="T3" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
@@ -594,17 +594,19 @@
       </c>
       <c r="T4" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="n">
+        <v>40909</v>
+      </c>
       <c r="I5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="T5" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="6">
       <c r="B6" s="4"/>
       <c r="C6" s="8"/>
       <c r="I6" s="0" t="s">
@@ -612,7 +614,7 @@
       </c>
       <c r="T6" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="B7" s="4"/>
       <c r="C7" s="8"/>
       <c r="I7" s="0" t="s">
@@ -620,7 +622,7 @@
       </c>
       <c r="T7" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -633,7 +635,7 @@
       </c>
       <c r="T8" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="9">
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
@@ -643,7 +645,7 @@
       </c>
       <c r="T9" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
       <c r="I10" s="0" t="s">
@@ -651,7 +653,7 @@
       </c>
       <c r="T10" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -662,7 +664,7 @@
       </c>
       <c r="T11" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -673,7 +675,7 @@
       </c>
       <c r="T12" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -684,7 +686,7 @@
       </c>
       <c r="T13" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
@@ -695,12 +697,12 @@
       </c>
       <c r="T14" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="T15" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>32</v>
       </c>
@@ -709,7 +711,7 @@
       </c>
       <c r="T16" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>34</v>
       </c>
@@ -718,7 +720,7 @@
       </c>
       <c r="T17" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>35</v>
       </c>
@@ -727,7 +729,7 @@
       </c>
       <c r="T18" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>36</v>
       </c>
@@ -759,49 +761,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM14"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="N1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="T3" activeCellId="0" pane="topLeft" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.19607843137255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.2156862745098"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.84705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.70980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.9098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.03921568627451"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.0549019607843"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3803921568627"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.5529411764706"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.0549019607843"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.721568627451"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.20392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.72941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.9490196078431"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.05882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9098039215686"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.078431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.7411764705882"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.72156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.22352941176471"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="4.69019607843137"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.078431372549"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.69803921568628"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1058823529412"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.71764705882353"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2196078431373"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.69803921568628"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2392156862745"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.71764705882353"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.87058823529412"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.0588235294118"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.7333333333333"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.8980392156863"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.3843137254902"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="11.2156862745098"/>
-    <col collapsed="false" hidden="false" max="38" min="33" style="0" width="8.37254901960784"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="27.9529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="8.37254901960784"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9372549019608"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.4039215686275"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="11.2352941176471"/>
+    <col collapsed="false" hidden="false" max="37" min="32" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="28.0117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
       <c r="A1" s="11" t="str">
         <f aca="false">DOC_SRC!C3</f>
         <v>ticker</v>
@@ -837,16 +838,15 @@
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
       <c r="A2" s="11" t="str">
         <f aca="false">DOC_SRC!C4</f>
         <v>coname</v>
@@ -887,9 +887,8 @@
       <c r="AC2" s="12"/>
       <c r="AD2" s="12"/>
       <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="A3" s="13" t="n">
         <v>40908</v>
       </c>
@@ -972,22 +971,19 @@
         <v>64</v>
       </c>
       <c r="AB3" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC3" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AD3" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE3" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF3" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="4">
       <c r="A4" s="14" t="s">
         <v>69</v>
       </c>
@@ -1067,28 +1063,25 @@
         <v>1</v>
       </c>
       <c r="AA4" s="16" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AB4" s="16" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AC4" s="16" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="AD4" s="16" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="AE4" s="16" t="n">
-        <v>400</v>
-      </c>
-      <c r="AF4" s="16" t="n">
         <v>500</v>
       </c>
-      <c r="AM4" s="0" t="s">
+      <c r="AL4" s="0" t="s">
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="5">
       <c r="A5" s="14" t="s">
         <v>78</v>
       </c>
@@ -1118,16 +1111,15 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
       <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="17"/>
       <c r="AD5" s="17"/>
       <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AM5" s="0" t="s">
+      <c r="AL5" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="6">
       <c r="A6" s="14" t="s">
         <v>80</v>
       </c>
@@ -1157,16 +1149,15 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="17"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="17"/>
       <c r="AD6" s="17"/>
       <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AM6" s="0" t="s">
+      <c r="AL6" s="0" t="s">
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="7">
       <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
@@ -1200,12 +1191,11 @@
       <c r="AC7" s="17"/>
       <c r="AD7" s="17"/>
       <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AM7" s="0" t="s">
+      <c r="AL7" s="0" t="s">
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="8">
       <c r="A8" s="14" t="s">
         <v>83</v>
       </c>
@@ -1239,23 +1229,22 @@
       <c r="AC8" s="17"/>
       <c r="AD8" s="17"/>
       <c r="AE8" s="17"/>
-      <c r="AF8" s="17"/>
-      <c r="AM8" s="0" t="s">
+      <c r="AL8" s="0" t="s">
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="9">
       <c r="A9" s="17"/>
+      <c r="AA9" s="17"/>
       <c r="AB9" s="17"/>
       <c r="AC9" s="17"/>
       <c r="AD9" s="17"/>
       <c r="AE9" s="17"/>
-      <c r="AF9" s="17"/>
-      <c r="AM9" s="0" t="s">
+      <c r="AL9" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="10">
       <c r="A10" s="14" t="s">
         <v>69</v>
       </c>
@@ -1335,28 +1324,25 @@
         <v>1</v>
       </c>
       <c r="AA10" s="16" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AB10" s="16" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AC10" s="16" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="AD10" s="16" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="AE10" s="16" t="n">
-        <v>400</v>
-      </c>
-      <c r="AF10" s="16" t="n">
         <v>500</v>
       </c>
-      <c r="AM10" s="0" t="s">
+      <c r="AL10" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="11">
       <c r="A11" s="14" t="s">
         <v>78</v>
       </c>
@@ -1386,16 +1372,15 @@
       <c r="Y11" s="17"/>
       <c r="Z11" s="17"/>
       <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="17"/>
       <c r="AD11" s="17"/>
       <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AM11" s="0" t="s">
+      <c r="AL11" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="12">
       <c r="A12" s="14" t="s">
         <v>80</v>
       </c>
@@ -1425,16 +1410,15 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
       <c r="AA12" s="17"/>
-      <c r="AB12" s="17"/>
-      <c r="AC12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="17"/>
       <c r="AD12" s="17"/>
       <c r="AE12" s="17"/>
-      <c r="AF12" s="17"/>
-      <c r="AM12" s="0" t="s">
+      <c r="AL12" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="13">
       <c r="A13" s="14" t="s">
         <v>1</v>
       </c>
@@ -1468,12 +1452,11 @@
       <c r="AC13" s="17"/>
       <c r="AD13" s="17"/>
       <c r="AE13" s="17"/>
-      <c r="AF13" s="17"/>
-      <c r="AM13" s="0" t="s">
+      <c r="AL13" s="0" t="s">
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="1" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="14">
       <c r="A14" s="14" t="s">
         <v>83</v>
       </c>
@@ -1507,8 +1490,7 @@
       <c r="AC14" s="17"/>
       <c r="AD14" s="17"/>
       <c r="AE14" s="17"/>
-      <c r="AF14" s="17"/>
-      <c r="AM14" s="0" t="s">
+      <c r="AL14" s="0" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1516,11 +1498,11 @@
   <mergeCells count="7">
     <mergeCell ref="B1:H2"/>
     <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:AA1"/>
-    <mergeCell ref="AB1:AF2"/>
+    <mergeCell ref="P1:Z1"/>
+    <mergeCell ref="AA1:AE2"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:AA2"/>
+    <mergeCell ref="P2:Z2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
new functional match fields added
</commit_message>
<xml_diff>
--- a/test/input/CompanyFiscalYearAndOneSheet.xlsx
+++ b/test/input/CompanyFiscalYearAndOneSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t>Input Value</t>
   </si>
@@ -178,16 +178,25 @@
     <t>Short Title</t>
   </si>
   <si>
-    <t>Functional Match</t>
-  </si>
-  <si>
-    <t>Functional Match 1</t>
-  </si>
-  <si>
-    <t>Functional Match 2</t>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>bod</t>
   </si>
   <si>
     <t>Founder</t>
+  </si>
+  <si>
+    <t>Transition Period</t>
   </si>
   <si>
     <t>Base Salary</t>
@@ -702,17 +711,17 @@
   </sheetPr>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5:E70"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -1445,7 +1454,7 @@
       <c r="D68" s="10"/>
       <c r="E68" s="24"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="69">
       <c r="A69" s="25" t="s">
         <v>39</v>
       </c>
@@ -1456,7 +1465,7 @@
       <c r="D69" s="10"/>
       <c r="E69" s="24"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="70">
       <c r="A70" s="29" t="s">
         <v>40</v>
       </c>
@@ -1492,11 +1501,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:E70 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.44313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1514,45 +1523,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL14"/>
+  <dimension ref="A1:AO14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="F4" activeCellId="1" pane="topLeft" sqref="A5:E70 F4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9176470588235"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.21960784313726"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.84705882352941"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.74901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.0274509803922"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9607843137255"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4470588235294"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6313725490196"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.24705882352941"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="4.69019607843137"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1843137254902"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.71764705882353"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.2980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.721568627451"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="8.10196078431373"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6509803921569"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9882352941176"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.0274509803922"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.4666666666667"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6509803921569"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1529411764706"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8196078431373"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.74117647058824"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.24705882352941"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="4.69019607843137"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.2235294117647"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.71764705882353"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.93725490196078"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.8117647058824"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.0156862745098"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.4509803921569"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="11.2862745098039"/>
-    <col collapsed="false" hidden="false" max="37" min="32" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="28.1490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.3176470588235"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.71764705882353"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.35294117647059"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.95686274509804"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="13.8313725490196"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.043137254902"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.4705882352941"/>
+    <col collapsed="false" hidden="false" max="34" min="33" style="0" width="11.3058823529412"/>
+    <col collapsed="false" hidden="false" max="40" min="35" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="28.2078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="42" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -1569,21 +1578,21 @@
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
       <c r="H1" s="33"/>
-      <c r="I1" s="33" t="s">
-        <v>45</v>
-      </c>
+      <c r="I1" s="33"/>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="L1" s="33" t="s">
+        <v>45</v>
+      </c>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
-      <c r="P1" s="33" t="s">
-        <v>46</v>
-      </c>
+      <c r="P1" s="33"/>
       <c r="Q1" s="33"/>
       <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
+      <c r="S1" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="T1" s="33"/>
       <c r="U1" s="33"/>
       <c r="V1" s="33"/>
@@ -1591,13 +1600,16 @@
       <c r="X1" s="33"/>
       <c r="Y1" s="33"/>
       <c r="Z1" s="33"/>
-      <c r="AA1" s="33" t="s">
-        <v>47</v>
-      </c>
+      <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
       <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
+      <c r="AD1" s="33" t="s">
+        <v>47</v>
+      </c>
       <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
       <c r="A2" s="32" t="str">
@@ -1611,23 +1623,23 @@
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
-      <c r="I2" s="33" t="s">
-        <v>48</v>
-      </c>
+      <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="L2" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="M2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33" t="s">
+      <c r="R2" s="33"/>
+      <c r="S2" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
       <c r="T2" s="33"/>
       <c r="U2" s="33"/>
       <c r="V2" s="33"/>
@@ -1640,6 +1652,9 @@
       <c r="AC2" s="33"/>
       <c r="AD2" s="33"/>
       <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="A3" s="34" t="n">
@@ -1682,19 +1697,19 @@
         <v>61</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="P3" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" s="35" t="s">
         <v>62</v>
-      </c>
-      <c r="Q3" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="35" t="s">
-        <v>64</v>
       </c>
       <c r="S3" s="35" t="s">
         <v>65</v>
@@ -1712,19 +1727,19 @@
         <v>69</v>
       </c>
       <c r="X3" s="35" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Y3" s="35" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="Z3" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AA3" s="35" t="s">
+      <c r="AB3" s="35" t="s">
         <v>71</v>
-      </c>
-      <c r="AB3" s="35" t="s">
-        <v>72</v>
       </c>
       <c r="AC3" s="35" t="s">
         <v>73</v>
@@ -1735,39 +1750,42 @@
       <c r="AE3" s="35" t="s">
         <v>75</v>
       </c>
+      <c r="AF3" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG3" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH3" s="35" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="4">
       <c r="A4" s="35" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="37" t="n">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="37" t="n">
         <v>1000</v>
       </c>
-      <c r="J4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="37" t="n">
+      <c r="M4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="N4" s="37" t="n">
@@ -1810,27 +1828,36 @@
         <v>1</v>
       </c>
       <c r="AA4" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="37" t="n">
         <v>100</v>
       </c>
-      <c r="AB4" s="37" t="n">
+      <c r="AE4" s="37" t="n">
         <v>200</v>
       </c>
-      <c r="AC4" s="37" t="n">
+      <c r="AF4" s="37" t="n">
         <v>300</v>
       </c>
-      <c r="AD4" s="37" t="n">
+      <c r="AG4" s="37" t="n">
         <v>400</v>
       </c>
-      <c r="AE4" s="37" t="n">
+      <c r="AH4" s="37" t="n">
         <v>500</v>
       </c>
-      <c r="AL4" s="0" t="s">
-        <v>81</v>
+      <c r="AO4" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="5">
       <c r="A5" s="35" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -1858,17 +1885,20 @@
       <c r="Y5" s="38"/>
       <c r="Z5" s="38"/>
       <c r="AA5" s="38"/>
-      <c r="AB5" s="39"/>
+      <c r="AB5" s="38"/>
       <c r="AC5" s="38"/>
       <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AL5" s="0" t="s">
-        <v>83</v>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AO5" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="6">
       <c r="A6" s="35" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" s="38"/>
@@ -1896,12 +1926,15 @@
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
       <c r="AA6" s="38"/>
-      <c r="AB6" s="39"/>
+      <c r="AB6" s="38"/>
       <c r="AC6" s="38"/>
       <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AL6" s="0" t="s">
-        <v>85</v>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AO6" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="7">
@@ -1938,13 +1971,16 @@
       <c r="AC7" s="38"/>
       <c r="AD7" s="38"/>
       <c r="AE7" s="38"/>
-      <c r="AL7" s="0" t="s">
-        <v>86</v>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="38"/>
+      <c r="AO7" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="8">
       <c r="A8" s="35" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -1976,52 +2012,56 @@
       <c r="AC8" s="38"/>
       <c r="AD8" s="38"/>
       <c r="AE8" s="38"/>
-      <c r="AL8" s="0" t="s">
-        <v>88</v>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AO8" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="9">
       <c r="A9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
       <c r="AD9" s="38"/>
       <c r="AE9" s="38"/>
-      <c r="AL9" s="0" t="s">
-        <v>89</v>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AO9" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="10">
       <c r="A10" s="35" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="37" t="n">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="37" t="n">
         <v>1000</v>
       </c>
-      <c r="J10" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="37" t="n">
-        <v>1</v>
-      </c>
       <c r="M10" s="37" t="n">
         <v>1</v>
       </c>
@@ -2065,27 +2105,36 @@
         <v>1</v>
       </c>
       <c r="AA10" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="37" t="n">
         <v>100</v>
       </c>
-      <c r="AB10" s="37" t="n">
+      <c r="AE10" s="37" t="n">
         <v>200</v>
       </c>
-      <c r="AC10" s="37" t="n">
+      <c r="AF10" s="37" t="n">
         <v>300</v>
       </c>
-      <c r="AD10" s="37" t="n">
+      <c r="AG10" s="37" t="n">
         <v>400</v>
       </c>
-      <c r="AE10" s="37" t="n">
+      <c r="AH10" s="37" t="n">
         <v>500</v>
       </c>
-      <c r="AL10" s="0" t="s">
-        <v>93</v>
+      <c r="AO10" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="11">
       <c r="A11" s="35" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2113,17 +2162,20 @@
       <c r="Y11" s="38"/>
       <c r="Z11" s="38"/>
       <c r="AA11" s="38"/>
-      <c r="AB11" s="39"/>
+      <c r="AB11" s="38"/>
       <c r="AC11" s="38"/>
       <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AL11" s="0" t="s">
-        <v>94</v>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AO11" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="12">
       <c r="A12" s="35" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -2151,12 +2203,15 @@
       <c r="Y12" s="38"/>
       <c r="Z12" s="38"/>
       <c r="AA12" s="38"/>
-      <c r="AB12" s="39"/>
+      <c r="AB12" s="38"/>
       <c r="AC12" s="38"/>
       <c r="AD12" s="38"/>
-      <c r="AE12" s="38"/>
-      <c r="AL12" s="0" t="s">
-        <v>95</v>
+      <c r="AE12" s="39"/>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38"/>
+      <c r="AO12" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="13">
@@ -2193,13 +2248,16 @@
       <c r="AC13" s="38"/>
       <c r="AD13" s="38"/>
       <c r="AE13" s="38"/>
-      <c r="AL13" s="0" t="s">
-        <v>96</v>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
+      <c r="AO13" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="14">
       <c r="A14" s="35" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -2231,19 +2289,22 @@
       <c r="AC14" s="38"/>
       <c r="AD14" s="38"/>
       <c r="AE14" s="38"/>
-      <c r="AL14" s="0" t="s">
-        <v>97</v>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AO14" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:H2"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:Z1"/>
-    <mergeCell ref="AA1:AE2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Z2"/>
+    <mergeCell ref="B1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:AC1"/>
+    <mergeCell ref="AD1:AH2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:AC2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>